<commit_message>
Adiciona código do projeto e .gitignore
</commit_message>
<xml_diff>
--- a/codigo_database.xlsx
+++ b/codigo_database.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
@@ -2622,6 +2622,23 @@
         </is>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>VDS2073</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>13/11/2025 11:56:43</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>6323</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>